<commit_message>
Implemented GEP with constant region mutation and inversion
</commit_message>
<xml_diff>
--- a/randomvsGEP.xlsx
+++ b/randomvsGEP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafael Stevenson\Desktop\Kuliah\Tesis S2\GEP_ForresterCase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6400B48A-1E1B-4F0A-9B6E-AD44287C3428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{332ACD54-EABA-4C3D-98F3-7C1868914DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="870" yWindow="1035" windowWidth="27000" windowHeight="14115" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>Run</t>
   </si>
@@ -56,6 +56,12 @@
   </si>
   <si>
     <t>n_perfect solution</t>
+  </si>
+  <si>
+    <t>GEP(pop25, gen40)</t>
+  </si>
+  <si>
+    <t>GEP(pop40, gen25)</t>
   </si>
 </sst>
 </file>
@@ -402,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,9 +421,11 @@
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -436,8 +444,20 @@
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -456,8 +476,17 @@
       <c r="F2" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>997.76899699820694</v>
+      </c>
+      <c r="I2">
+        <v>1000</v>
+      </c>
+      <c r="J2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -474,8 +503,17 @@
       <c r="F3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>999.27344704546101</v>
+      </c>
+      <c r="I3">
+        <v>1000</v>
+      </c>
+      <c r="J3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -492,8 +530,17 @@
         <v>997.37773564997303</v>
       </c>
       <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>1000</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>998.14113464749403</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -508,8 +555,14 @@
         <v>999.09378359774303</v>
       </c>
       <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>997.76899699820694</v>
+      </c>
+      <c r="I5">
+        <v>997.76899699820694</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -528,8 +581,11 @@
       <c r="F6" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>999.79219766162396</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -546,8 +602,14 @@
       <c r="F7" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <v>1000</v>
+      </c>
+      <c r="J7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -562,8 +624,14 @@
         <v>997.54305803694604</v>
       </c>
       <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <v>1000</v>
+      </c>
+      <c r="J8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -578,8 +646,11 @@
         <v>998.60049180392696</v>
       </c>
       <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <v>997.54305803694604</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -596,8 +667,11 @@
         <v>999.89215105881999</v>
       </c>
       <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <v>998.30575172668398</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -612,8 +686,11 @@
         <v>998.30575172668398</v>
       </c>
       <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <v>997.76899699820694</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -630,8 +707,11 @@
         <v>998.09722387962302</v>
       </c>
       <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <v>999.92484796702797</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -647,7 +727,7 @@
       </c>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -667,7 +747,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -683,7 +763,7 @@
       </c>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -840,7 +920,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:C24 E1:E24">
+  <conditionalFormatting sqref="B1:C24 E1:E24 G1:J1">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>